<commit_message>
harmoniza nomes das colunas em caixa alta
</commit_message>
<xml_diff>
--- a/data-raw/fonte_stn.xlsx
+++ b/data-raw/fonte_stn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Projects/matriz-fonte-stn-dadosmg/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fjunior/Projects/matriz-fonte-stn-dadosmg/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8AB990-D51F-D74E-87D7-F410A5AF47AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE13DC11-5E9B-CD48-924B-8F827037520D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{7F3748C7-0441-5749-8552-FD6593F21ACD}"/>
   </bookViews>
@@ -586,25 +586,25 @@
     <t>Controle dos recursos cuja aplicação seja vinculada e não tenha sido enquadrado em outras especificações.</t>
   </si>
   <si>
-    <t>codigo</t>
-  </si>
-  <si>
-    <t>descricao</t>
-  </si>
-  <si>
-    <t>interpretacao</t>
-  </si>
-  <si>
-    <t>dt_inicio_vigencia</t>
-  </si>
-  <si>
-    <t>dt_fim_vigencia</t>
-  </si>
-  <si>
     <t>2023-01-01</t>
   </si>
   <si>
     <t>9999-12-01</t>
+  </si>
+  <si>
+    <t>FONTE_STN_COD</t>
+  </si>
+  <si>
+    <t>FONTE_STN_DESCRICAO</t>
+  </si>
+  <si>
+    <t>INTERPRETACAO</t>
+  </si>
+  <si>
+    <t>DT_INICIO_VIGENCIA</t>
+  </si>
+  <si>
+    <t>DT_FIM_VIGENCIA</t>
   </si>
 </sst>
 </file>
@@ -659,9 +659,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -987,29 +986,29 @@
     <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="2" max="2" width="93.1640625" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E1" s="2" t="s">
         <v>174</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>500</v>
       </c>
       <c r="B2" t="s">
@@ -1018,15 +1017,15 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>176</v>
+      <c r="D2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>501</v>
       </c>
       <c r="B3" t="s">
@@ -1035,11 +1034,11 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>176</v>
+      <c r="D3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1052,15 +1051,15 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>176</v>
+      <c r="D4" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>540</v>
       </c>
       <c r="B5" t="s">
@@ -1069,15 +1068,15 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>176</v>
+      <c r="D5" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>541</v>
       </c>
       <c r="B6" t="s">
@@ -1086,15 +1085,15 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>176</v>
+      <c r="D6" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>542</v>
       </c>
       <c r="B7" t="s">
@@ -1103,15 +1102,15 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>176</v>
+      <c r="D7" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>543</v>
       </c>
       <c r="B8" t="s">
@@ -1120,15 +1119,15 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>176</v>
+      <c r="D8" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>544</v>
       </c>
       <c r="B9" t="s">
@@ -1137,15 +1136,15 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>176</v>
+      <c r="D9" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>550</v>
       </c>
       <c r="B10" t="s">
@@ -1154,15 +1153,15 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>176</v>
+      <c r="D10" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>551</v>
       </c>
       <c r="B11" t="s">
@@ -1171,15 +1170,15 @@
       <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>176</v>
+      <c r="D11" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>552</v>
       </c>
       <c r="B12" t="s">
@@ -1188,15 +1187,15 @@
       <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>176</v>
+      <c r="D12" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>553</v>
       </c>
       <c r="B13" t="s">
@@ -1205,15 +1204,15 @@
       <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>176</v>
+      <c r="D13" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>569</v>
       </c>
       <c r="B14" t="s">
@@ -1222,15 +1221,15 @@
       <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>176</v>
+      <c r="D14" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>570</v>
       </c>
       <c r="B15" t="s">
@@ -1239,15 +1238,15 @@
       <c r="C15" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>176</v>
+      <c r="D15" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>571</v>
       </c>
       <c r="B16" t="s">
@@ -1256,15 +1255,15 @@
       <c r="C16" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>176</v>
+      <c r="D16" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>572</v>
       </c>
       <c r="B17" t="s">
@@ -1273,15 +1272,15 @@
       <c r="C17" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>176</v>
+      <c r="D17" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>573</v>
       </c>
       <c r="B18" t="s">
@@ -1290,15 +1289,15 @@
       <c r="C18" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>176</v>
+      <c r="D18" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>574</v>
       </c>
       <c r="B19" t="s">
@@ -1307,15 +1306,15 @@
       <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>176</v>
+      <c r="D19" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>575</v>
       </c>
       <c r="B20" t="s">
@@ -1324,15 +1323,15 @@
       <c r="C20" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>176</v>
+      <c r="D20" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>576</v>
       </c>
       <c r="B21" t="s">
@@ -1341,15 +1340,15 @@
       <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>176</v>
+      <c r="D21" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>599</v>
       </c>
       <c r="B22" t="s">
@@ -1358,15 +1357,15 @@
       <c r="C22" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>176</v>
+      <c r="D22" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>600</v>
       </c>
       <c r="B23" t="s">
@@ -1375,15 +1374,15 @@
       <c r="C23" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>176</v>
+      <c r="D23" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>601</v>
       </c>
       <c r="B24" t="s">
@@ -1392,15 +1391,15 @@
       <c r="C24" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>176</v>
+      <c r="D24" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+      <c r="A25">
         <v>602</v>
       </c>
       <c r="B25" t="s">
@@ -1409,15 +1408,15 @@
       <c r="C25" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>176</v>
+      <c r="D25" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+      <c r="A26">
         <v>603</v>
       </c>
       <c r="B26" t="s">
@@ -1426,15 +1425,15 @@
       <c r="C26" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>176</v>
+      <c r="D26" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+      <c r="A27">
         <v>604</v>
       </c>
       <c r="B27" t="s">
@@ -1443,15 +1442,15 @@
       <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>176</v>
+      <c r="D27" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+      <c r="A28">
         <v>621</v>
       </c>
       <c r="B28" t="s">
@@ -1460,15 +1459,15 @@
       <c r="C28" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>176</v>
+      <c r="D28" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
+      <c r="A29">
         <v>622</v>
       </c>
       <c r="B29" t="s">
@@ -1477,15 +1476,15 @@
       <c r="C29" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>176</v>
+      <c r="D29" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
+      <c r="A30">
         <v>631</v>
       </c>
       <c r="B30" t="s">
@@ -1494,15 +1493,15 @@
       <c r="C30" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>176</v>
+      <c r="D30" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
+      <c r="A31">
         <v>632</v>
       </c>
       <c r="B31" t="s">
@@ -1511,15 +1510,15 @@
       <c r="C31" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>176</v>
+      <c r="D31" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
+      <c r="A32">
         <v>633</v>
       </c>
       <c r="B32" t="s">
@@ -1528,15 +1527,15 @@
       <c r="C32" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>176</v>
+      <c r="D32" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
+      <c r="A33">
         <v>634</v>
       </c>
       <c r="B33" t="s">
@@ -1545,15 +1544,15 @@
       <c r="C33" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>176</v>
+      <c r="D33" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
+      <c r="A34">
         <v>635</v>
       </c>
       <c r="B34" t="s">
@@ -1562,15 +1561,15 @@
       <c r="C34" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>176</v>
+      <c r="D34" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
+      <c r="A35">
         <v>636</v>
       </c>
       <c r="B35" t="s">
@@ -1579,15 +1578,15 @@
       <c r="C35" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>176</v>
+      <c r="D35" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
+      <c r="A36">
         <v>659</v>
       </c>
       <c r="B36" t="s">
@@ -1596,15 +1595,15 @@
       <c r="C36" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>176</v>
+      <c r="D36" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
+      <c r="A37">
         <v>660</v>
       </c>
       <c r="B37" t="s">
@@ -1613,15 +1612,15 @@
       <c r="C37" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>176</v>
+      <c r="D37" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
+      <c r="A38">
         <v>661</v>
       </c>
       <c r="B38" t="s">
@@ -1630,15 +1629,15 @@
       <c r="C38" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>176</v>
+      <c r="D38" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
+      <c r="A39">
         <v>662</v>
       </c>
       <c r="B39" t="s">
@@ -1647,15 +1646,15 @@
       <c r="C39" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>176</v>
+      <c r="D39" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
+      <c r="A40">
         <v>665</v>
       </c>
       <c r="B40" t="s">
@@ -1664,15 +1663,15 @@
       <c r="C40" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>176</v>
+      <c r="D40" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
+      <c r="A41">
         <v>669</v>
       </c>
       <c r="B41" t="s">
@@ -1681,15 +1680,15 @@
       <c r="C41" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>176</v>
+      <c r="D41" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
+      <c r="A42">
         <v>700</v>
       </c>
       <c r="B42" t="s">
@@ -1698,15 +1697,15 @@
       <c r="C42" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>176</v>
+      <c r="D42" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
+      <c r="A43">
         <v>701</v>
       </c>
       <c r="B43" t="s">
@@ -1715,15 +1714,15 @@
       <c r="C43" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>176</v>
+      <c r="D43" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
+      <c r="A44">
         <v>702</v>
       </c>
       <c r="B44" t="s">
@@ -1732,15 +1731,15 @@
       <c r="C44" t="s">
         <v>85</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>176</v>
+      <c r="D44" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
+      <c r="A45">
         <v>703</v>
       </c>
       <c r="B45" t="s">
@@ -1749,15 +1748,15 @@
       <c r="C45" t="s">
         <v>87</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>176</v>
+      <c r="D45" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
+      <c r="A46">
         <v>704</v>
       </c>
       <c r="B46" t="s">
@@ -1766,15 +1765,15 @@
       <c r="C46" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>176</v>
+      <c r="D46" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
+      <c r="A47">
         <v>705</v>
       </c>
       <c r="B47" t="s">
@@ -1783,15 +1782,15 @@
       <c r="C47" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>176</v>
+      <c r="D47" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
+      <c r="A48">
         <v>706</v>
       </c>
       <c r="B48" t="s">
@@ -1800,15 +1799,15 @@
       <c r="C48" t="s">
         <v>93</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>176</v>
+      <c r="D48" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
+      <c r="A49">
         <v>707</v>
       </c>
       <c r="B49" t="s">
@@ -1817,15 +1816,15 @@
       <c r="C49" t="s">
         <v>95</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>176</v>
+      <c r="D49" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
+      <c r="A50">
         <v>708</v>
       </c>
       <c r="B50" t="s">
@@ -1834,15 +1833,15 @@
       <c r="C50" t="s">
         <v>97</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>176</v>
+      <c r="D50" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
+      <c r="A51">
         <v>709</v>
       </c>
       <c r="B51" t="s">
@@ -1851,15 +1850,15 @@
       <c r="C51" t="s">
         <v>99</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>176</v>
+      <c r="D51" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
+      <c r="A52">
         <v>710</v>
       </c>
       <c r="B52" t="s">
@@ -1868,15 +1867,15 @@
       <c r="C52" t="s">
         <v>101</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>176</v>
+      <c r="D52" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
+      <c r="A53">
         <v>711</v>
       </c>
       <c r="B53" t="s">
@@ -1885,15 +1884,15 @@
       <c r="C53" t="s">
         <v>103</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>176</v>
+      <c r="D53" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
+      <c r="A54">
         <v>712</v>
       </c>
       <c r="B54" t="s">
@@ -1902,15 +1901,15 @@
       <c r="C54" t="s">
         <v>105</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>176</v>
+      <c r="D54" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
+      <c r="A55">
         <v>713</v>
       </c>
       <c r="B55" t="s">
@@ -1919,15 +1918,15 @@
       <c r="C55" t="s">
         <v>107</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>176</v>
+      <c r="D55" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
+      <c r="A56">
         <v>714</v>
       </c>
       <c r="B56" t="s">
@@ -1936,15 +1935,15 @@
       <c r="C56" t="s">
         <v>109</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>176</v>
+      <c r="D56" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
+      <c r="A57">
         <v>715</v>
       </c>
       <c r="B57" t="s">
@@ -1953,15 +1952,15 @@
       <c r="C57" t="s">
         <v>111</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>176</v>
+      <c r="D57" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
+      <c r="A58">
         <v>716</v>
       </c>
       <c r="B58" t="s">
@@ -1970,15 +1969,15 @@
       <c r="C58" t="s">
         <v>113</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>176</v>
+      <c r="D58" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
+      <c r="A59">
         <v>717</v>
       </c>
       <c r="B59" t="s">
@@ -1987,15 +1986,15 @@
       <c r="C59" t="s">
         <v>115</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>176</v>
+      <c r="D59" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
+      <c r="A60">
         <v>718</v>
       </c>
       <c r="B60" t="s">
@@ -2004,15 +2003,15 @@
       <c r="C60" t="s">
         <v>117</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>176</v>
+      <c r="D60" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
+      <c r="A61">
         <v>719</v>
       </c>
       <c r="B61" t="s">
@@ -2021,15 +2020,15 @@
       <c r="C61" t="s">
         <v>119</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>176</v>
+      <c r="D61" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
+      <c r="A62">
         <v>749</v>
       </c>
       <c r="B62" t="s">
@@ -2038,15 +2037,15 @@
       <c r="C62" t="s">
         <v>121</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>176</v>
+      <c r="D62" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
+      <c r="A63">
         <v>750</v>
       </c>
       <c r="B63" t="s">
@@ -2055,15 +2054,15 @@
       <c r="C63" t="s">
         <v>123</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>176</v>
+      <c r="D63" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
+      <c r="A64">
         <v>751</v>
       </c>
       <c r="B64" t="s">
@@ -2072,15 +2071,15 @@
       <c r="C64" t="s">
         <v>125</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>176</v>
+      <c r="D64" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
+      <c r="A65">
         <v>752</v>
       </c>
       <c r="B65" t="s">
@@ -2089,15 +2088,15 @@
       <c r="C65" t="s">
         <v>127</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>176</v>
+      <c r="D65" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
+      <c r="A66">
         <v>753</v>
       </c>
       <c r="B66" t="s">
@@ -2106,15 +2105,15 @@
       <c r="C66" t="s">
         <v>129</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>176</v>
+      <c r="D66" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="1">
+      <c r="A67">
         <v>754</v>
       </c>
       <c r="B67" t="s">
@@ -2123,15 +2122,15 @@
       <c r="C67" t="s">
         <v>131</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>176</v>
+      <c r="D67" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="1">
+      <c r="A68">
         <v>755</v>
       </c>
       <c r="B68" t="s">
@@ -2140,15 +2139,15 @@
       <c r="C68" t="s">
         <v>133</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>176</v>
+      <c r="D68" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="1">
+      <c r="A69">
         <v>756</v>
       </c>
       <c r="B69" t="s">
@@ -2157,15 +2156,15 @@
       <c r="C69" t="s">
         <v>135</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>176</v>
+      <c r="D69" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="1">
+      <c r="A70">
         <v>757</v>
       </c>
       <c r="B70" t="s">
@@ -2174,15 +2173,15 @@
       <c r="C70" t="s">
         <v>137</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>176</v>
+      <c r="D70" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="1">
+      <c r="A71">
         <v>758</v>
       </c>
       <c r="B71" t="s">
@@ -2191,15 +2190,15 @@
       <c r="C71" t="s">
         <v>139</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>176</v>
+      <c r="D71" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="1">
+      <c r="A72">
         <v>759</v>
       </c>
       <c r="B72" t="s">
@@ -2208,15 +2207,15 @@
       <c r="C72" t="s">
         <v>141</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>176</v>
+      <c r="D72" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="1">
+      <c r="A73">
         <v>760</v>
       </c>
       <c r="B73" t="s">
@@ -2225,15 +2224,15 @@
       <c r="C73" t="s">
         <v>143</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>176</v>
+      <c r="D73" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="1">
+      <c r="A74">
         <v>761</v>
       </c>
       <c r="B74" t="s">
@@ -2242,15 +2241,15 @@
       <c r="C74" t="s">
         <v>145</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>176</v>
+      <c r="D74" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="1">
+      <c r="A75">
         <v>799</v>
       </c>
       <c r="B75" t="s">
@@ -2259,15 +2258,15 @@
       <c r="C75" t="s">
         <v>147</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>176</v>
+      <c r="D75" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="1">
+      <c r="A76">
         <v>800</v>
       </c>
       <c r="B76" t="s">
@@ -2276,15 +2275,15 @@
       <c r="C76" t="s">
         <v>149</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>176</v>
+      <c r="D76" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="1">
+      <c r="A77">
         <v>801</v>
       </c>
       <c r="B77" t="s">
@@ -2293,15 +2292,15 @@
       <c r="C77" t="s">
         <v>151</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>176</v>
+      <c r="D77" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="1">
+      <c r="A78">
         <v>802</v>
       </c>
       <c r="B78" t="s">
@@ -2310,15 +2309,15 @@
       <c r="C78" t="s">
         <v>153</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>176</v>
+      <c r="D78" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="1">
+      <c r="A79">
         <v>803</v>
       </c>
       <c r="B79" t="s">
@@ -2327,15 +2326,15 @@
       <c r="C79" t="s">
         <v>155</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>176</v>
+      <c r="D79" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="1">
+      <c r="A80">
         <v>860</v>
       </c>
       <c r="B80" t="s">
@@ -2344,15 +2343,15 @@
       <c r="C80" t="s">
         <v>157</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>176</v>
+      <c r="D80" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="1">
+      <c r="A81">
         <v>861</v>
       </c>
       <c r="B81" t="s">
@@ -2361,15 +2360,15 @@
       <c r="C81" t="s">
         <v>159</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>176</v>
+      <c r="D81" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" s="1">
+      <c r="A82">
         <v>862</v>
       </c>
       <c r="B82" t="s">
@@ -2378,15 +2377,15 @@
       <c r="C82" t="s">
         <v>161</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>176</v>
+      <c r="D82" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="1">
+      <c r="A83">
         <v>869</v>
       </c>
       <c r="B83" t="s">
@@ -2395,15 +2394,15 @@
       <c r="C83" t="s">
         <v>163</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>176</v>
+      <c r="D83" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" s="1">
+      <c r="A84">
         <v>880</v>
       </c>
       <c r="B84" t="s">
@@ -2412,15 +2411,15 @@
       <c r="C84" t="s">
         <v>165</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>176</v>
+      <c r="D84" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" s="1">
+      <c r="A85">
         <v>898</v>
       </c>
       <c r="B85" t="s">
@@ -2429,15 +2428,15 @@
       <c r="C85" t="s">
         <v>167</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>176</v>
+      <c r="D85" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" s="1">
+      <c r="A86">
         <v>899</v>
       </c>
       <c r="B86" t="s">
@@ -2446,11 +2445,11 @@
       <c r="C86" t="s">
         <v>169</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>176</v>
+      <c r="D86" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>